<commit_message>
Documentacion de la primera iteracion
</commit_message>
<xml_diff>
--- a/Documentacion de Requerimientos/Estimación de Tiempo (Esfuerzo) y Costo Italia Pizza.xlsx
+++ b/Documentacion de Requerimientos/Estimación de Tiempo (Esfuerzo) y Costo Italia Pizza.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27421"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uvmx-my.sharepoint.com/personal/zs21013909_estudiantes_uv_mx/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos C#\ItalianPizza\Italia-Pizza-Documentacion\Documentacion de Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA1CB649-DBE2-4F60-ACF5-2CD1A255DD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50801D69-4584-4DE9-B2A9-E19DB53E57E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="752" firstSheet="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25840" windowHeight="13933" tabRatio="752" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inf.Gral" sheetId="38" r:id="rId1"/>
@@ -842,11 +842,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="51">
+  <fonts count="51" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1730,7 +1730,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="43" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="47" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="47" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="221">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1786,7 +1786,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1918,13 +1918,13 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="36" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="36" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2029,7 +2029,7 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2070,7 +2070,7 @@
     <xf numFmtId="0" fontId="24" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="29" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="29" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="8" fillId="8" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2115,29 +2115,29 @@
     <xf numFmtId="0" fontId="18" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="38" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="38" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="37" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="37" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="41" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="41" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="48" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="24" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="24" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="48" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="49" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="44" fontId="49" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="37" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2155,18 +2155,51 @@
     <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2187,39 +2220,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3025,24 +3025,24 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="10.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="10.7" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="3" width="33" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="1"/>
+    <col min="4" max="4" width="25.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="67" customFormat="1" ht="37.5" customHeight="1">
+    <row r="1" spans="1:4" s="67" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="68"/>
       <c r="B1" s="66"/>
     </row>
-    <row r="2" spans="1:4" s="27" customFormat="1" ht="28.9">
+    <row r="2" spans="1:4" s="27" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
@@ -3050,13 +3050,13 @@
       <c r="C2" s="32"/>
       <c r="D2" s="26"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" s="4" customFormat="1" ht="13.9">
+    <row r="4" spans="1:4" s="4" customFormat="1" ht="13.35" x14ac:dyDescent="0.25">
       <c r="A4" s="122" t="s">
         <v>1</v>
       </c>
@@ -3066,7 +3066,7 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" s="4" customFormat="1" ht="13.9">
+    <row r="5" spans="1:4" s="4" customFormat="1" ht="13.35" x14ac:dyDescent="0.25">
       <c r="A5" s="122" t="s">
         <v>3</v>
       </c>
@@ -3076,12 +3076,12 @@
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" s="4" customFormat="1" ht="6" customHeight="1">
+    <row r="6" spans="1:4" s="4" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" s="28" customFormat="1" ht="21">
+    <row r="7" spans="1:4" s="28" customFormat="1" ht="20.7" x14ac:dyDescent="0.35">
       <c r="A7" s="188" t="s">
         <v>5</v>
       </c>
@@ -3089,7 +3089,7 @@
       <c r="C7" s="189"/>
       <c r="D7" s="189"/>
     </row>
-    <row r="8" spans="1:4" s="29" customFormat="1" ht="21">
+    <row r="8" spans="1:4" s="29" customFormat="1" ht="20.7" x14ac:dyDescent="0.35">
       <c r="A8" s="30" t="s">
         <v>6</v>
       </c>
@@ -3103,127 +3103,127 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="4" customFormat="1" ht="13.9">
+    <row r="9" spans="1:4" s="4" customFormat="1" ht="13.35" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="9"/>
       <c r="D9" s="10"/>
     </row>
-    <row r="10" spans="1:4" s="4" customFormat="1" ht="13.9">
+    <row r="10" spans="1:4" s="4" customFormat="1" ht="13.35" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
     </row>
-    <row r="11" spans="1:4" s="4" customFormat="1" ht="13.9">
+    <row r="11" spans="1:4" s="4" customFormat="1" ht="13.35" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
     </row>
-    <row r="12" spans="1:4" s="4" customFormat="1" ht="13.9">
+    <row r="12" spans="1:4" s="4" customFormat="1" ht="13.35" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:4" s="4" customFormat="1" ht="13.9">
+    <row r="13" spans="1:4" s="4" customFormat="1" ht="13.35" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
     </row>
-    <row r="14" spans="1:4" s="4" customFormat="1" ht="13.9">
+    <row r="14" spans="1:4" s="4" customFormat="1" ht="13.35" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="9"/>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="1:4" s="4" customFormat="1" ht="13.9">
+    <row r="15" spans="1:4" s="4" customFormat="1" ht="13.35" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:4" s="4" customFormat="1" ht="13.9">
+    <row r="16" spans="1:4" s="4" customFormat="1" ht="13.35" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:4" s="4" customFormat="1" ht="13.9">
+    <row r="17" spans="1:4" s="4" customFormat="1" ht="13.35" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="9"/>
       <c r="D17" s="10"/>
     </row>
-    <row r="18" spans="1:4" s="4" customFormat="1" ht="13.9">
+    <row r="18" spans="1:4" s="4" customFormat="1" ht="13.35" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="1:4" s="4" customFormat="1" ht="13.9">
+    <row r="19" spans="1:4" s="4" customFormat="1" ht="13.35" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="9"/>
       <c r="D19" s="10"/>
     </row>
-    <row r="20" spans="1:4" s="4" customFormat="1" ht="13.9">
+    <row r="20" spans="1:4" s="4" customFormat="1" ht="13.35" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="9"/>
       <c r="D20" s="10"/>
     </row>
-    <row r="21" spans="1:4" s="4" customFormat="1" ht="13.9">
+    <row r="21" spans="1:4" s="4" customFormat="1" ht="13.35" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="1:4" s="4" customFormat="1" ht="13.9">
+    <row r="22" spans="1:4" s="4" customFormat="1" ht="13.35" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
     </row>
-    <row r="23" spans="1:4" s="4" customFormat="1" ht="13.9">
+    <row r="23" spans="1:4" s="4" customFormat="1" ht="13.35" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="9"/>
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:4" s="4" customFormat="1" ht="13.9">
+    <row r="24" spans="1:4" s="4" customFormat="1" ht="13.35" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="9"/>
       <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="1:4" s="4" customFormat="1" ht="13.9">
+    <row r="25" spans="1:4" s="4" customFormat="1" ht="13.35" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="1:4" s="4" customFormat="1" ht="13.9">
+    <row r="26" spans="1:4" s="4" customFormat="1" ht="13.35" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="8"/>
       <c r="C26" s="9"/>
       <c r="D26" s="10"/>
     </row>
-    <row r="27" spans="1:4" s="4" customFormat="1" ht="13.9">
+    <row r="27" spans="1:4" s="4" customFormat="1" ht="13.35" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
       <c r="D27" s="10"/>
     </row>
-    <row r="28" spans="1:4" s="4" customFormat="1" ht="13.9">
+    <row r="28" spans="1:4" s="4" customFormat="1" ht="13.35" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="8"/>
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
     </row>
-    <row r="29" spans="1:4" s="4" customFormat="1" ht="13.9">
+    <row r="29" spans="1:4" s="4" customFormat="1" ht="13.35" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="8"/>
       <c r="C29" s="9"/>
@@ -3247,16 +3247,16 @@
       <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="15.35" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="11" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" style="11" customWidth="1"/>
+    <col min="1" max="1" width="1.75" style="11" customWidth="1"/>
+    <col min="2" max="2" width="25.875" style="11" customWidth="1"/>
     <col min="3" max="3" width="62" style="11" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="11"/>
+    <col min="4" max="16384" width="11.375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="32.25" customHeight="1"/>
-    <row r="2" spans="1:17" s="33" customFormat="1" ht="25.9">
+    <row r="1" spans="1:17" ht="32.35" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:17" s="33" customFormat="1" ht="26" x14ac:dyDescent="0.45">
       <c r="A2" s="71"/>
       <c r="B2" s="190" t="s">
         <v>10</v>
@@ -3279,7 +3279,7 @@
       <c r="P2" s="73"/>
       <c r="Q2" s="73"/>
     </row>
-    <row r="4" spans="1:17" s="33" customFormat="1" ht="25.9">
+    <row r="4" spans="1:17" s="33" customFormat="1" ht="26" x14ac:dyDescent="0.45">
       <c r="A4" s="71"/>
       <c r="B4" s="72" t="s">
         <v>12</v>
@@ -3300,12 +3300,12 @@
       <c r="P4" s="73"/>
       <c r="Q4" s="73"/>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="23.45">
+    <row r="7" spans="1:17" ht="23.35" x14ac:dyDescent="0.4">
       <c r="B7" s="38" t="s">
         <v>14</v>
       </c>
@@ -3313,7 +3313,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="72">
+    <row r="8" spans="1:17" ht="76.7" x14ac:dyDescent="0.3">
       <c r="B8" s="37" t="s">
         <v>15</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="72">
+    <row r="9" spans="1:17" ht="76.7" x14ac:dyDescent="0.3">
       <c r="B9" s="37" t="s">
         <v>17</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="72">
+    <row r="10" spans="1:17" ht="76.7" x14ac:dyDescent="0.3">
       <c r="B10" s="37" t="s">
         <v>19</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="33" customFormat="1" ht="25.9">
+    <row r="12" spans="1:17" s="33" customFormat="1" ht="26" x14ac:dyDescent="0.45">
       <c r="A12" s="71"/>
       <c r="B12" s="72" t="s">
         <v>21</v>
@@ -3358,17 +3358,17 @@
       <c r="P12" s="73"/>
       <c r="Q12" s="73"/>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B13" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B14" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="24" thickBot="1">
+    <row r="16" spans="1:17" ht="24" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B16" s="38" t="s">
         <v>24</v>
       </c>
@@ -3376,7 +3376,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B17" s="49" t="s">
         <v>25</v>
       </c>
@@ -3384,7 +3384,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B18" s="48" t="s">
         <v>27</v>
       </c>
@@ -3392,7 +3392,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B19" s="48" t="s">
         <v>29</v>
       </c>
@@ -3400,7 +3400,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="19"/>
       <c r="B20" s="35" t="s">
         <v>31</v>
@@ -3409,7 +3409,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="51"/>
       <c r="B21" s="35" t="s">
         <v>33</v>
@@ -3418,7 +3418,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="19"/>
       <c r="B22" s="35" t="s">
         <v>35</v>
@@ -3427,7 +3427,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="19"/>
       <c r="B23" s="35" t="s">
         <v>37</v>
@@ -3436,7 +3436,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="19"/>
       <c r="B24" s="35" t="s">
         <v>39</v>
@@ -3445,7 +3445,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
       <c r="B25" s="35" t="s">
         <v>41</v>
@@ -3454,7 +3454,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="35" t="s">
         <v>43</v>
@@ -3463,7 +3463,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
       <c r="B27" s="34" t="s">
         <v>45</v>
@@ -3472,7 +3472,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B28" s="45" t="s">
         <v>47</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="15" thickBot="1">
+    <row r="29" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="46" t="s">
         <v>49</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="33" customFormat="1" ht="25.9">
+    <row r="31" spans="1:17" s="33" customFormat="1" ht="26" x14ac:dyDescent="0.45">
       <c r="A31" s="71"/>
       <c r="B31" s="72" t="s">
         <v>51</v>
@@ -3509,17 +3509,17 @@
       <c r="P31" s="73"/>
       <c r="Q31" s="73"/>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B32" s="11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="2:3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="2:3" ht="47.45" thickBot="1">
+    <row r="35" spans="2:3" ht="47.35" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B35" s="53" t="s">
         <v>53</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="2:3">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B36" s="49" t="s">
         <v>54</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="2:3">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B37" s="37" t="s">
         <v>56</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="2:3">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B38" s="44" t="s">
         <v>58</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="2:3">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" s="48" t="s">
         <v>60</v>
       </c>
@@ -3559,7 +3559,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="2:3">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B40" s="37" t="s">
         <v>62</v>
       </c>
@@ -3567,7 +3567,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="2:3">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B41" s="44" t="s">
         <v>64</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="2:3">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B42" s="44" t="s">
         <v>66</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="2:3" ht="15" thickBot="1">
+    <row r="43" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B43" s="57" t="s">
         <v>68</v>
       </c>
@@ -3612,65 +3612,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:H42"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="113" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView showGridLines="0" topLeftCell="A31" zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="15.35" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="5.25" style="11" customWidth="1"/>
     <col min="2" max="2" width="17" style="11" customWidth="1"/>
-    <col min="3" max="3" width="59.7109375" style="11" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="11" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="11" customWidth="1"/>
-    <col min="7" max="7" width="46.140625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="11"/>
+    <col min="3" max="3" width="59.75" style="11" customWidth="1"/>
+    <col min="4" max="4" width="13.25" style="11" customWidth="1"/>
+    <col min="5" max="5" width="10.125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="11.875" style="11" customWidth="1"/>
+    <col min="7" max="7" width="46.125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="6.75" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.375" style="11"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="18">
+    <row r="2" spans="2:8" ht="18.7" x14ac:dyDescent="0.35">
       <c r="B2" s="69" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="33" customHeight="1">
-      <c r="B3" s="210" t="s">
+    <row r="3" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="192" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="210"/>
-      <c r="D3" s="210"/>
-      <c r="E3" s="210"/>
-      <c r="F3" s="210"/>
-      <c r="G3" s="210"/>
-      <c r="H3" s="210"/>
-    </row>
-    <row r="4" spans="2:8">
-      <c r="B4" s="211" t="s">
+      <c r="C3" s="192"/>
+      <c r="D3" s="192"/>
+      <c r="E3" s="192"/>
+      <c r="F3" s="192"/>
+      <c r="G3" s="192"/>
+      <c r="H3" s="192"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="193" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="211"/>
-      <c r="D4" s="211"/>
-      <c r="E4" s="211"/>
-      <c r="F4" s="211"/>
-      <c r="G4" s="211"/>
-      <c r="H4" s="211"/>
-    </row>
-    <row r="5" spans="2:8">
+      <c r="C4" s="193"/>
+      <c r="D4" s="193"/>
+      <c r="E4" s="193"/>
+      <c r="F4" s="193"/>
+      <c r="G4" s="193"/>
+      <c r="H4" s="193"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="120"/>
     </row>
-    <row r="8" spans="2:8" ht="23.45">
-      <c r="B8" s="205" t="s">
+    <row r="8" spans="2:8" ht="23.35" x14ac:dyDescent="0.4">
+      <c r="B8" s="196" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="206"/>
-      <c r="D8" s="206"/>
-      <c r="E8" s="206"/>
-      <c r="F8" s="206"/>
-      <c r="G8" s="206"/>
-      <c r="H8" s="207"/>
-    </row>
-    <row r="9" spans="2:8" ht="18">
+      <c r="C8" s="197"/>
+      <c r="D8" s="197"/>
+      <c r="E8" s="197"/>
+      <c r="F8" s="197"/>
+      <c r="G8" s="197"/>
+      <c r="H8" s="198"/>
+    </row>
+    <row r="9" spans="2:8" ht="18.7" x14ac:dyDescent="0.35">
       <c r="B9" s="99"/>
       <c r="C9" s="100"/>
       <c r="D9" s="100"/>
@@ -3684,7 +3684,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="28.9">
+    <row r="10" spans="2:8" ht="30.7" x14ac:dyDescent="0.3">
       <c r="B10" s="101" t="s">
         <v>53</v>
       </c>
@@ -3700,12 +3700,12 @@
       <c r="F10" s="101" t="s">
         <v>76</v>
       </c>
-      <c r="G10" s="208" t="s">
+      <c r="G10" s="203" t="s">
         <v>77</v>
       </c>
-      <c r="H10" s="209"/>
-    </row>
-    <row r="11" spans="2:8">
+      <c r="H10" s="204"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="14" t="s">
         <v>25</v>
       </c>
@@ -3722,12 +3722,12 @@
         <f t="shared" ref="F11:F23" si="0">E11*D11</f>
         <v>2</v>
       </c>
-      <c r="G11" s="203" t="s">
+      <c r="G11" s="201" t="s">
         <v>78</v>
       </c>
-      <c r="H11" s="204"/>
-    </row>
-    <row r="12" spans="2:8">
+      <c r="H11" s="202"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="16" t="s">
         <v>27</v>
       </c>
@@ -3749,7 +3749,7 @@
       </c>
       <c r="H12" s="195"/>
     </row>
-    <row r="13" spans="2:8">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="16" t="s">
         <v>29</v>
       </c>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="H13" s="195"/>
     </row>
-    <row r="14" spans="2:8">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="16" t="s">
         <v>31</v>
       </c>
@@ -3793,7 +3793,7 @@
       </c>
       <c r="H14" s="195"/>
     </row>
-    <row r="15" spans="2:8">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="16" t="s">
         <v>33</v>
       </c>
@@ -3815,7 +3815,7 @@
       </c>
       <c r="H15" s="195"/>
     </row>
-    <row r="16" spans="2:8">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="16" t="s">
         <v>35</v>
       </c>
@@ -3837,7 +3837,7 @@
       </c>
       <c r="H16" s="19"/>
     </row>
-    <row r="17" spans="2:8">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="16" t="s">
         <v>37</v>
       </c>
@@ -3859,7 +3859,7 @@
       </c>
       <c r="H17" s="195"/>
     </row>
-    <row r="18" spans="2:8">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="16" t="s">
         <v>39</v>
       </c>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="2:8">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="16" t="s">
         <v>41</v>
       </c>
@@ -3903,7 +3903,7 @@
       </c>
       <c r="H19" s="195"/>
     </row>
-    <row r="20" spans="2:8">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="16" t="s">
         <v>43</v>
       </c>
@@ -3925,7 +3925,7 @@
       </c>
       <c r="H20" s="195"/>
     </row>
-    <row r="21" spans="2:8">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="16" t="s">
         <v>45</v>
       </c>
@@ -3947,7 +3947,7 @@
       </c>
       <c r="H21" s="195"/>
     </row>
-    <row r="22" spans="2:8">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="16" t="s">
         <v>47</v>
       </c>
@@ -3969,7 +3969,7 @@
       </c>
       <c r="H22" s="195"/>
     </row>
-    <row r="23" spans="2:8">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="17" t="s">
         <v>49</v>
       </c>
@@ -3991,7 +3991,7 @@
       </c>
       <c r="H23" s="195"/>
     </row>
-    <row r="24" spans="2:8">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="104"/>
       <c r="C24" s="105"/>
       <c r="D24" s="105"/>
@@ -4005,18 +4005,18 @@
       <c r="G24" s="105"/>
       <c r="H24" s="107"/>
     </row>
-    <row r="27" spans="2:8" ht="23.45">
-      <c r="B27" s="205" t="s">
+    <row r="27" spans="2:8" ht="23.35" x14ac:dyDescent="0.4">
+      <c r="B27" s="196" t="s">
         <v>92</v>
       </c>
-      <c r="C27" s="206"/>
-      <c r="D27" s="206"/>
-      <c r="E27" s="206"/>
-      <c r="F27" s="206"/>
-      <c r="G27" s="206"/>
-      <c r="H27" s="207"/>
-    </row>
-    <row r="28" spans="2:8" ht="18">
+      <c r="C27" s="197"/>
+      <c r="D27" s="197"/>
+      <c r="E27" s="197"/>
+      <c r="F27" s="197"/>
+      <c r="G27" s="197"/>
+      <c r="H27" s="198"/>
+    </row>
+    <row r="28" spans="2:8" ht="18.7" x14ac:dyDescent="0.35">
       <c r="B28" s="100"/>
       <c r="C28" s="100"/>
       <c r="D28" s="100"/>
@@ -4030,7 +4030,7 @@
         <v>0.72499999999999998</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="28.9">
+    <row r="29" spans="2:8" ht="30.7" x14ac:dyDescent="0.3">
       <c r="B29" s="123" t="s">
         <v>94</v>
       </c>
@@ -4046,12 +4046,12 @@
       <c r="F29" s="123" t="s">
         <v>76</v>
       </c>
-      <c r="G29" s="212" t="s">
+      <c r="G29" s="199" t="s">
         <v>77</v>
       </c>
-      <c r="H29" s="213"/>
-    </row>
-    <row r="30" spans="2:8">
+      <c r="H29" s="200"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" s="14" t="s">
         <v>54</v>
       </c>
@@ -4068,10 +4068,10 @@
         <f t="shared" ref="F30:F37" si="1">E30*D30</f>
         <v>4.5</v>
       </c>
-      <c r="G30" s="203"/>
-      <c r="H30" s="204"/>
-    </row>
-    <row r="31" spans="2:8">
+      <c r="G30" s="201"/>
+      <c r="H30" s="202"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" s="16" t="s">
         <v>56</v>
       </c>
@@ -4091,7 +4091,7 @@
       <c r="G31" s="194"/>
       <c r="H31" s="195"/>
     </row>
-    <row r="32" spans="2:8">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B32" s="16" t="s">
         <v>58</v>
       </c>
@@ -4111,7 +4111,7 @@
       <c r="G32" s="194"/>
       <c r="H32" s="195"/>
     </row>
-    <row r="33" spans="2:8">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B33" s="16" t="s">
         <v>60</v>
       </c>
@@ -4131,7 +4131,7 @@
       <c r="G33" s="194"/>
       <c r="H33" s="195"/>
     </row>
-    <row r="34" spans="2:8">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B34" s="16" t="s">
         <v>62</v>
       </c>
@@ -4151,7 +4151,7 @@
       <c r="G34" s="194"/>
       <c r="H34" s="195"/>
     </row>
-    <row r="35" spans="2:8">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B35" s="16" t="s">
         <v>64</v>
       </c>
@@ -4170,7 +4170,7 @@
       </c>
       <c r="H35" s="19"/>
     </row>
-    <row r="36" spans="2:8">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B36" s="16" t="s">
         <v>66</v>
       </c>
@@ -4190,7 +4190,7 @@
       <c r="G36" s="194"/>
       <c r="H36" s="195"/>
     </row>
-    <row r="37" spans="2:8">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B37" s="16" t="s">
         <v>68</v>
       </c>
@@ -4209,7 +4209,7 @@
       </c>
       <c r="H37" s="19"/>
     </row>
-    <row r="38" spans="2:8">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B38" s="128"/>
       <c r="C38" s="129"/>
       <c r="D38" s="130"/>
@@ -4223,57 +4223,45 @@
       <c r="G38" s="130"/>
       <c r="H38" s="132"/>
     </row>
-    <row r="40" spans="2:8">
-      <c r="B40" s="196" t="s">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B40" s="207" t="s">
         <v>96</v>
       </c>
-      <c r="C40" s="197"/>
-      <c r="F40" s="200" t="s">
+      <c r="C40" s="208"/>
+      <c r="F40" s="211" t="s">
         <v>97</v>
       </c>
-      <c r="G40" s="201"/>
-      <c r="H40" s="201"/>
-    </row>
-    <row r="41" spans="2:8" ht="60" customHeight="1">
-      <c r="B41" s="198" t="s">
+      <c r="G40" s="212"/>
+      <c r="H40" s="212"/>
+    </row>
+    <row r="41" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="209" t="s">
         <v>98</v>
       </c>
-      <c r="C41" s="199"/>
-      <c r="F41" s="198" t="s">
+      <c r="C41" s="210"/>
+      <c r="F41" s="209" t="s">
         <v>99</v>
       </c>
-      <c r="G41" s="202"/>
-      <c r="H41" s="202"/>
-    </row>
-    <row r="42" spans="2:8" ht="43.15">
+      <c r="G41" s="213"/>
+      <c r="H41" s="213"/>
+    </row>
+    <row r="42" spans="2:8" ht="46" x14ac:dyDescent="0.3">
       <c r="B42" s="133" t="s">
         <v>100</v>
       </c>
       <c r="C42" s="152">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F42" s="134" t="s">
         <v>101</v>
       </c>
-      <c r="G42" s="192">
+      <c r="G42" s="205">
         <v>4</v>
       </c>
-      <c r="H42" s="193"/>
+      <c r="H42" s="206"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G10:H10"/>
     <mergeCell ref="G42:H42"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="B40:C40"/>
@@ -4290,6 +4278,18 @@
     <mergeCell ref="G33:H33"/>
     <mergeCell ref="G34:H34"/>
     <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="G29:H29"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="1">
@@ -4305,28 +4305,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:G40"/>
+  <dimension ref="B1:G31"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="15.35" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" style="13" customWidth="1"/>
-    <col min="3" max="3" width="70.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="4.75" style="13" customWidth="1"/>
+    <col min="3" max="3" width="70.625" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="11" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" style="13" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="13" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="11"/>
-    <col min="9" max="9" width="12.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="11"/>
+    <col min="5" max="5" width="7.375" style="13" customWidth="1"/>
+    <col min="6" max="6" width="10.75" style="13" customWidth="1"/>
+    <col min="7" max="7" width="15.75" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.375" style="11"/>
+    <col min="9" max="9" width="12.125" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="33.75" customHeight="1"/>
-    <row r="2" spans="2:7" ht="25.9">
+    <row r="1" spans="2:7" ht="33.85" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" ht="26" x14ac:dyDescent="0.45">
       <c r="B2" s="214" t="s">
         <v>102</v>
       </c>
@@ -4336,7 +4336,7 @@
       <c r="F2" s="214"/>
       <c r="G2" s="214"/>
     </row>
-    <row r="3" spans="2:7" ht="18">
+    <row r="3" spans="2:7" ht="18.7" x14ac:dyDescent="0.35">
       <c r="B3" s="109"/>
       <c r="C3" s="110"/>
       <c r="D3" s="111"/>
@@ -4349,7 +4349,7 @@
         <v>197.63499999999996</v>
       </c>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="109" t="s">
         <v>104</v>
       </c>
@@ -4369,7 +4369,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="12">
         <v>1</v>
       </c>
@@ -4391,7 +4391,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:7">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="12">
         <v>2</v>
       </c>
@@ -4413,7 +4413,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:7">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" s="12">
         <v>3</v>
       </c>
@@ -4435,7 +4435,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:7">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="12">
         <v>4</v>
       </c>
@@ -4457,7 +4457,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:7">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" s="12">
         <v>5</v>
       </c>
@@ -4479,7 +4479,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:7">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" s="12">
         <v>6</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="15">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" s="12">
         <v>7</v>
       </c>
@@ -4523,7 +4523,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:7">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" s="12">
         <v>8</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:7">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13" s="12">
         <v>9</v>
       </c>
@@ -4567,7 +4567,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="2:7">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14" s="12">
         <v>10</v>
       </c>
@@ -4589,7 +4589,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:7">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" s="12">
         <v>11</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:7">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" s="12">
         <v>12</v>
       </c>
@@ -4633,7 +4633,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:7">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="12">
         <f>B16+1</f>
         <v>13</v>
@@ -4656,7 +4656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="12">
         <f t="shared" ref="B18:B31" si="2">B17+1</f>
         <v>14</v>
@@ -4679,7 +4679,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="2:7">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="12">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -4702,7 +4702,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="12">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -4725,7 +4725,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="2:7">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="12">
         <f t="shared" si="2"/>
         <v>17</v>
@@ -4748,7 +4748,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="12">
         <f t="shared" si="2"/>
         <v>18</v>
@@ -4771,7 +4771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="2:7">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="12">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -4794,7 +4794,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="2:7">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" s="12">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -4817,7 +4817,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="2:7">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="12">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -4840,7 +4840,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="2:7">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" s="12">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -4863,7 +4863,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="2:7">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" s="12">
         <f t="shared" si="2"/>
         <v>23</v>
@@ -4886,7 +4886,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="2:7">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B28" s="12">
         <f t="shared" si="2"/>
         <v>24</v>
@@ -4909,7 +4909,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="2:7">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B29" s="12">
         <f t="shared" si="2"/>
         <v>25</v>
@@ -4932,7 +4932,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="2:7">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30" s="12">
         <f t="shared" si="2"/>
         <v>26</v>
@@ -4955,7 +4955,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="2:7">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B31" s="12">
         <f t="shared" si="2"/>
         <v>27</v>
@@ -4978,13 +4978,6 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" ht="15"/>
-    <row r="35" ht="15"/>
-    <row r="36" ht="15"/>
-    <row r="37" ht="15"/>
-    <row r="38" ht="15"/>
-    <row r="39" ht="15"/>
-    <row r="40" ht="15"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:G2"/>
@@ -5008,26 +5001,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:N53"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="G9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="15.35" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.5703125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" style="13" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="7.25" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="10.25" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.75" style="13" customWidth="1"/>
+    <col min="6" max="6" width="22.375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.75" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" style="11" customWidth="1"/>
-    <col min="9" max="9" width="27.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.25" style="11" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="12" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="11.42578125" style="11"/>
+    <col min="12" max="16384" width="11.375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="36" customHeight="1">
+    <row r="1" spans="2:14" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -5042,7 +5035,7 @@
       <c r="M1" s="24"/>
       <c r="N1" s="25"/>
     </row>
-    <row r="2" spans="2:14" ht="15.6">
+    <row r="2" spans="2:14" ht="16" x14ac:dyDescent="0.3">
       <c r="B2" s="24"/>
       <c r="C2" s="138" t="s">
         <v>138</v>
@@ -5063,7 +5056,7 @@
       <c r="M2" s="24"/>
       <c r="N2" s="25"/>
     </row>
-    <row r="3" spans="2:14">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" s="24"/>
       <c r="C3" s="138" t="s">
         <v>140</v>
@@ -5076,7 +5069,7 @@
       </c>
       <c r="F3" s="151">
         <f>ROUNDUP(E7/D2,0)</f>
-        <v>198</v>
+        <v>396</v>
       </c>
       <c r="G3" s="120"/>
       <c r="H3" s="120"/>
@@ -5087,21 +5080,21 @@
       <c r="M3" s="24"/>
       <c r="N3" s="25"/>
     </row>
-    <row r="4" spans="2:14" ht="15" customHeight="1">
+    <row r="4" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="24"/>
       <c r="C4" s="138" t="s">
         <v>142</v>
       </c>
       <c r="D4" s="144">
         <f>'Factor de complejidad Téc y Amb'!C42</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E4" s="138" t="s">
         <v>143</v>
       </c>
       <c r="F4" s="150">
         <f>F3/D3</f>
-        <v>39.6</v>
+        <v>79.2</v>
       </c>
       <c r="G4" s="120"/>
       <c r="H4" s="159"/>
@@ -5112,7 +5105,7 @@
       <c r="M4" s="24"/>
       <c r="N4" s="25"/>
     </row>
-    <row r="5" spans="2:14" ht="15" customHeight="1">
+    <row r="5" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="24"/>
       <c r="C5" s="138" t="s">
         <v>144</v>
@@ -5126,7 +5119,7 @@
       </c>
       <c r="F5" s="150">
         <f>F4/4</f>
-        <v>9.9</v>
+        <v>19.8</v>
       </c>
       <c r="G5" s="120"/>
       <c r="H5" s="120"/>
@@ -5137,7 +5130,7 @@
       <c r="M5" s="24"/>
       <c r="N5" s="25"/>
     </row>
-    <row r="6" spans="2:14" ht="25.9">
+    <row r="6" spans="2:14" ht="26" x14ac:dyDescent="0.45">
       <c r="B6" s="218" t="s">
         <v>146</v>
       </c>
@@ -5149,13 +5142,13 @@
       <c r="H6" s="219"/>
       <c r="I6" s="219"/>
     </row>
-    <row r="7" spans="2:14" ht="21">
+    <row r="7" spans="2:14" ht="20.7" x14ac:dyDescent="0.35">
       <c r="B7" s="59"/>
       <c r="C7" s="60"/>
       <c r="D7" s="60"/>
       <c r="E7" s="114">
         <f>SUM(E9+E15+E27+E37+E43+E31)</f>
-        <v>1185.8099999999997</v>
+        <v>2371.6199999999994</v>
       </c>
       <c r="F7" s="169" t="s">
         <v>147</v>
@@ -5164,7 +5157,7 @@
       <c r="H7" s="59"/>
       <c r="I7" s="59"/>
     </row>
-    <row r="8" spans="2:14" ht="15.6">
+    <row r="8" spans="2:14" ht="16" x14ac:dyDescent="0.3">
       <c r="B8" s="61" t="s">
         <v>104</v>
       </c>
@@ -5188,7 +5181,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="2:14" ht="15.6">
+    <row r="9" spans="2:14" ht="16" x14ac:dyDescent="0.3">
       <c r="B9" s="74">
         <v>1</v>
       </c>
@@ -5200,7 +5193,7 @@
       </c>
       <c r="E9" s="164">
         <f>$E$31*D9</f>
-        <v>39.526999999999994</v>
+        <v>79.053999999999988</v>
       </c>
       <c r="F9" s="88">
         <v>1</v>
@@ -5211,10 +5204,10 @@
       <c r="H9" s="172"/>
       <c r="I9" s="172">
         <f>SUM(I10:I14)</f>
-        <v>3379.2345081967205</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" ht="15.6">
+        <v>6758.4690163934411</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="16" x14ac:dyDescent="0.3">
       <c r="B10" s="63">
         <v>1.1000000000000001</v>
       </c>
@@ -5226,7 +5219,7 @@
       </c>
       <c r="E10" s="165">
         <f>$E$9*D10</f>
-        <v>3.9526999999999997</v>
+        <v>7.9053999999999993</v>
       </c>
       <c r="F10" s="63">
         <v>1</v>
@@ -5240,10 +5233,10 @@
       </c>
       <c r="I10" s="171">
         <f t="shared" ref="I10:I14" si="0">E10*H10*F10</f>
-        <v>229.22420081967209</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" ht="15.6">
+        <v>458.44840163934418</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" ht="16" x14ac:dyDescent="0.3">
       <c r="B11" s="63">
         <v>1.2</v>
       </c>
@@ -5255,7 +5248,7 @@
       </c>
       <c r="E11" s="165">
         <f t="shared" ref="E11" si="1">$E$9*D11</f>
-        <v>11.858099999999999</v>
+        <v>23.716199999999997</v>
       </c>
       <c r="F11" s="63">
         <v>1</v>
@@ -5269,10 +5262,10 @@
       </c>
       <c r="I11" s="171">
         <f t="shared" si="0"/>
-        <v>984.12510245901626</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" ht="15.6">
+        <v>1968.2502049180325</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="16" x14ac:dyDescent="0.3">
       <c r="B12" s="63">
         <v>1.3</v>
       </c>
@@ -5284,7 +5277,7 @@
       </c>
       <c r="E12" s="165">
         <f t="shared" ref="E12:E14" si="2">$E$9*D12</f>
-        <v>15.810799999999999</v>
+        <v>31.621599999999997</v>
       </c>
       <c r="F12" s="63">
         <v>1</v>
@@ -5298,10 +5291,10 @@
       </c>
       <c r="I12" s="171">
         <f t="shared" si="0"/>
-        <v>1312.1668032786883</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" ht="15.6">
+        <v>2624.3336065573767</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="16" x14ac:dyDescent="0.3">
       <c r="B13" s="153">
         <v>1.4</v>
       </c>
@@ -5313,7 +5306,7 @@
       </c>
       <c r="E13" s="165">
         <f t="shared" si="2"/>
-        <v>3.9526999999999997</v>
+        <v>7.9053999999999993</v>
       </c>
       <c r="F13" s="63">
         <v>1</v>
@@ -5327,10 +5320,10 @@
       </c>
       <c r="I13" s="171">
         <f t="shared" si="0"/>
-        <v>328.04170081967209</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" ht="15.6">
+        <v>656.08340163934417</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="16" x14ac:dyDescent="0.3">
       <c r="B14" s="153">
         <v>1.5</v>
       </c>
@@ -5342,7 +5335,7 @@
       </c>
       <c r="E14" s="165">
         <f t="shared" si="2"/>
-        <v>3.9526999999999997</v>
+        <v>7.9053999999999993</v>
       </c>
       <c r="F14" s="63">
         <v>1</v>
@@ -5356,10 +5349,10 @@
       </c>
       <c r="I14" s="171">
         <f t="shared" si="0"/>
-        <v>525.67670081967208</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" ht="15.6">
+        <v>1051.3534016393442</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="16" x14ac:dyDescent="0.3">
       <c r="B15" s="74">
         <v>2</v>
       </c>
@@ -5371,7 +5364,7 @@
       </c>
       <c r="E15" s="164">
         <f>$E$31*D15</f>
-        <v>118.58099999999997</v>
+        <v>237.16199999999995</v>
       </c>
       <c r="F15" s="88">
         <v>1</v>
@@ -5382,10 +5375,10 @@
       <c r="H15" s="172"/>
       <c r="I15" s="172">
         <f>SUM(I16:I26)</f>
-        <v>16801.809928278682</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" ht="15.6">
+        <v>33603.619856557365</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" ht="16" x14ac:dyDescent="0.3">
       <c r="B16" s="63">
         <v>2.1</v>
       </c>
@@ -5397,7 +5390,7 @@
       </c>
       <c r="E16" s="165">
         <f>$E$15*D16</f>
-        <v>17.787149999999997</v>
+        <v>35.574299999999994</v>
       </c>
       <c r="F16" s="63">
         <v>1</v>
@@ -5411,10 +5404,10 @@
       </c>
       <c r="I16" s="171">
         <f t="shared" ref="I16:I26" si="3">E16*H16*F16</f>
-        <v>2365.5451536885244</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" ht="15.6">
+        <v>4731.0903073770487</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="16" x14ac:dyDescent="0.3">
       <c r="B17" s="63">
         <v>2.2000000000000002</v>
       </c>
@@ -5426,7 +5419,7 @@
       </c>
       <c r="E17" s="165">
         <f>$E$15*D17</f>
-        <v>17.787149999999997</v>
+        <v>35.574299999999994</v>
       </c>
       <c r="F17" s="63">
         <v>1</v>
@@ -5440,10 +5433,10 @@
       </c>
       <c r="I17" s="171">
         <f t="shared" si="3"/>
-        <v>2365.5451536885244</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="15.6">
+        <v>4731.0903073770487</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="16" x14ac:dyDescent="0.3">
       <c r="B18" s="63">
         <v>2.2999999999999998</v>
       </c>
@@ -5455,7 +5448,7 @@
       </c>
       <c r="E18" s="165">
         <f t="shared" ref="E18:E22" si="4">$E$15*D18</f>
-        <v>17.787149999999997</v>
+        <v>35.574299999999994</v>
       </c>
       <c r="F18" s="63">
         <v>1</v>
@@ -5469,10 +5462,10 @@
       </c>
       <c r="I18" s="171">
         <f t="shared" si="3"/>
-        <v>2365.5451536885244</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" ht="15.6">
+        <v>4731.0903073770487</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="16" x14ac:dyDescent="0.3">
       <c r="B19" s="63">
         <v>2.4</v>
       </c>
@@ -5484,7 +5477,7 @@
       </c>
       <c r="E19" s="165">
         <f t="shared" si="4"/>
-        <v>5.9290499999999993</v>
+        <v>11.858099999999999</v>
       </c>
       <c r="F19" s="63">
         <v>1</v>
@@ -5498,10 +5491,10 @@
       </c>
       <c r="I19" s="171">
         <f t="shared" ref="I19:I20" si="5">E19*H19*F19</f>
-        <v>788.51505122950812</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" ht="15.6">
+        <v>1577.0301024590162</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="16" x14ac:dyDescent="0.3">
       <c r="B20" s="63">
         <v>2.5</v>
       </c>
@@ -5513,7 +5506,7 @@
       </c>
       <c r="E20" s="165">
         <f t="shared" si="4"/>
-        <v>11.858099999999999</v>
+        <v>23.716199999999997</v>
       </c>
       <c r="F20" s="63">
         <v>1</v>
@@ -5527,10 +5520,10 @@
       </c>
       <c r="I20" s="171">
         <f t="shared" si="5"/>
-        <v>1577.0301024590162</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" ht="15.6">
+        <v>3154.0602049180325</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="16" x14ac:dyDescent="0.3">
       <c r="B21" s="63">
         <v>2.6</v>
       </c>
@@ -5542,7 +5535,7 @@
       </c>
       <c r="E21" s="165">
         <f t="shared" si="4"/>
-        <v>5.9290499999999993</v>
+        <v>11.858099999999999</v>
       </c>
       <c r="F21" s="63">
         <v>1</v>
@@ -5556,10 +5549,10 @@
       </c>
       <c r="I21" s="171">
         <f t="shared" si="3"/>
-        <v>788.51505122950812</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" ht="15.6">
+        <v>1577.0301024590162</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="16" x14ac:dyDescent="0.3">
       <c r="B22" s="63">
         <v>2.7</v>
       </c>
@@ -5571,7 +5564,7 @@
       </c>
       <c r="E22" s="165">
         <f t="shared" si="4"/>
-        <v>11.858099999999999</v>
+        <v>23.716199999999997</v>
       </c>
       <c r="F22" s="63">
         <v>1</v>
@@ -5585,10 +5578,10 @@
       </c>
       <c r="I22" s="171">
         <f t="shared" si="3"/>
-        <v>984.12510245901626</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" ht="15.6">
+        <v>1968.2502049180325</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="16" x14ac:dyDescent="0.3">
       <c r="B23" s="63">
         <v>2.8</v>
       </c>
@@ -5600,7 +5593,7 @@
       </c>
       <c r="E23" s="165">
         <f t="shared" ref="E23:E26" si="6">$E$15*D23</f>
-        <v>11.858099999999999</v>
+        <v>23.716199999999997</v>
       </c>
       <c r="F23" s="63">
         <v>1</v>
@@ -5614,10 +5607,10 @@
       </c>
       <c r="I23" s="171">
         <f t="shared" si="3"/>
-        <v>1577.0301024590162</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" ht="15.6">
+        <v>3154.0602049180325</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="16" x14ac:dyDescent="0.3">
       <c r="B24" s="63">
         <v>2.9</v>
       </c>
@@ -5629,7 +5622,7 @@
       </c>
       <c r="E24" s="165">
         <f t="shared" si="6"/>
-        <v>5.9290499999999993</v>
+        <v>11.858099999999999</v>
       </c>
       <c r="F24" s="63">
         <v>1</v>
@@ -5643,10 +5636,10 @@
       </c>
       <c r="I24" s="171">
         <f t="shared" si="3"/>
-        <v>788.51505122950812</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" ht="15.6">
+        <v>1577.0301024590162</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="16" x14ac:dyDescent="0.3">
       <c r="B25" s="65">
         <v>2.1</v>
       </c>
@@ -5658,7 +5651,7 @@
       </c>
       <c r="E25" s="165">
         <f t="shared" si="6"/>
-        <v>5.9290499999999993</v>
+        <v>11.858099999999999</v>
       </c>
       <c r="F25" s="63">
         <v>1</v>
@@ -5672,10 +5665,10 @@
       </c>
       <c r="I25" s="171">
         <f t="shared" si="3"/>
-        <v>788.51505122950812</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" ht="15.6">
+        <v>1577.0301024590162</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" ht="16" x14ac:dyDescent="0.3">
       <c r="B26" s="65">
         <v>2.11</v>
       </c>
@@ -5687,7 +5680,7 @@
       </c>
       <c r="E26" s="165">
         <f t="shared" si="6"/>
-        <v>5.9290499999999993</v>
+        <v>11.858099999999999</v>
       </c>
       <c r="F26" s="63">
         <v>4</v>
@@ -5701,10 +5694,10 @@
       </c>
       <c r="I26" s="171">
         <f t="shared" si="3"/>
-        <v>2412.9289549180326</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" ht="15.6">
+        <v>4825.8579098360651</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="16" x14ac:dyDescent="0.3">
       <c r="B27" s="74">
         <v>3</v>
       </c>
@@ -5716,7 +5709,7 @@
       </c>
       <c r="E27" s="164">
         <f>$E$31*D27</f>
-        <v>79.053999999999988</v>
+        <v>158.10799999999998</v>
       </c>
       <c r="F27" s="88">
         <v>1</v>
@@ -5727,10 +5720,10 @@
       <c r="H27" s="172"/>
       <c r="I27" s="172">
         <f>SUM(I28:I36)</f>
-        <v>336957.95524590154</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" ht="15.6">
+        <v>673915.91049180308</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="16" x14ac:dyDescent="0.3">
       <c r="B28" s="63">
         <v>3.1</v>
       </c>
@@ -5742,7 +5735,7 @@
       </c>
       <c r="E28" s="165">
         <f>$E$27*D28</f>
-        <v>7.9053999999999993</v>
+        <v>15.810799999999999</v>
       </c>
       <c r="F28" s="76">
         <v>1</v>
@@ -5756,10 +5749,10 @@
       </c>
       <c r="I28" s="171">
         <f t="shared" ref="I28:I36" si="7">E28*H28*F28</f>
-        <v>656.08340163934417</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" ht="15.6">
+        <v>1312.1668032786883</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="16" x14ac:dyDescent="0.3">
       <c r="B29" s="63">
         <v>3.2</v>
       </c>
@@ -5771,7 +5764,7 @@
       </c>
       <c r="E29" s="165">
         <f>$E$27*D29</f>
-        <v>7.9053999999999993</v>
+        <v>15.810799999999999</v>
       </c>
       <c r="F29" s="76">
         <v>1</v>
@@ -5785,10 +5778,10 @@
       </c>
       <c r="I29" s="171">
         <f t="shared" si="7"/>
-        <v>310.22215163934419</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" ht="15.6">
+        <v>620.44430327868838</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" ht="16" x14ac:dyDescent="0.3">
       <c r="B30" s="63">
         <v>3.5</v>
       </c>
@@ -5800,7 +5793,7 @@
       </c>
       <c r="E30" s="165">
         <f>$E$27*D30</f>
-        <v>3.9526999999999997</v>
+        <v>7.9053999999999993</v>
       </c>
       <c r="F30" s="76">
         <v>1</v>
@@ -5814,10 +5807,10 @@
       </c>
       <c r="I30" s="171">
         <f t="shared" si="7"/>
-        <v>525.67670081967208</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" s="137" customFormat="1" ht="15.6">
+        <v>1051.3534016393442</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" s="137" customFormat="1" ht="16" x14ac:dyDescent="0.3">
       <c r="B31" s="63">
         <v>3.6</v>
       </c>
@@ -5827,7 +5820,7 @@
       <c r="D31" s="161"/>
       <c r="E31" s="168">
         <f>D4*D5</f>
-        <v>790.53999999999985</v>
+        <v>1581.0799999999997</v>
       </c>
       <c r="F31" s="76">
         <v>4</v>
@@ -5841,10 +5834,10 @@
       </c>
       <c r="I31" s="171">
         <f t="shared" si="7"/>
-        <v>321723.86065573763</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" ht="15.6">
+        <v>643447.72131147527</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" ht="16" x14ac:dyDescent="0.3">
       <c r="B32" s="63">
         <v>3.7</v>
       </c>
@@ -5856,7 +5849,7 @@
       </c>
       <c r="E32" s="165">
         <f>$E$27*D32</f>
-        <v>11.858099999999999</v>
+        <v>23.716199999999997</v>
       </c>
       <c r="F32" s="76">
         <v>4</v>
@@ -5870,10 +5863,10 @@
       </c>
       <c r="I32" s="171">
         <f t="shared" si="7"/>
-        <v>4825.8579098360651</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" ht="15.6">
+        <v>9651.7158196721302</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" ht="16" x14ac:dyDescent="0.3">
       <c r="B33" s="63">
         <v>3.9</v>
       </c>
@@ -5885,7 +5878,7 @@
       </c>
       <c r="E33" s="165">
         <f>$E$27*D33</f>
-        <v>11.858099999999999</v>
+        <v>23.716199999999997</v>
       </c>
       <c r="F33" s="76">
         <v>4</v>
@@ -5899,10 +5892,10 @@
       </c>
       <c r="I33" s="171">
         <f t="shared" si="7"/>
-        <v>4825.8579098360651</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" ht="15.6">
+        <v>9651.7158196721302</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" ht="16" x14ac:dyDescent="0.3">
       <c r="B34" s="65">
         <v>3.1</v>
       </c>
@@ -5914,7 +5907,7 @@
       </c>
       <c r="E34" s="165">
         <f>$E$27*D34</f>
-        <v>15.810799999999999</v>
+        <v>31.621599999999997</v>
       </c>
       <c r="F34" s="76">
         <v>2</v>
@@ -5928,10 +5921,10 @@
       </c>
       <c r="I34" s="171">
         <f t="shared" si="7"/>
-        <v>1240.8886065573768</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" ht="15.6">
+        <v>2481.7772131147535</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" ht="16" x14ac:dyDescent="0.3">
       <c r="B35" s="65">
         <v>3.11</v>
       </c>
@@ -5943,7 +5936,7 @@
       </c>
       <c r="E35" s="165">
         <f>$E$27*D35</f>
-        <v>15.810799999999999</v>
+        <v>31.621599999999997</v>
       </c>
       <c r="F35" s="76">
         <v>2</v>
@@ -5957,10 +5950,10 @@
       </c>
       <c r="I35" s="171">
         <f t="shared" si="7"/>
-        <v>1240.8886065573768</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" ht="15.6">
+        <v>2481.7772131147535</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" ht="16" x14ac:dyDescent="0.3">
       <c r="B36" s="65">
         <v>3.12</v>
       </c>
@@ -5972,7 +5965,7 @@
       </c>
       <c r="E36" s="165">
         <f>$E$27*D36</f>
-        <v>3.9526999999999997</v>
+        <v>7.9053999999999993</v>
       </c>
       <c r="F36" s="76">
         <v>4</v>
@@ -5986,10 +5979,10 @@
       </c>
       <c r="I36" s="171">
         <f t="shared" si="7"/>
-        <v>1608.6193032786884</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" ht="15.6">
+        <v>3217.2386065573769</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" ht="16" x14ac:dyDescent="0.3">
       <c r="B37" s="74">
         <v>4</v>
       </c>
@@ -6001,7 +5994,7 @@
       </c>
       <c r="E37" s="164">
         <f>$E$31*D37</f>
-        <v>79.053999999999988</v>
+        <v>158.10799999999998</v>
       </c>
       <c r="F37" s="88">
         <v>1</v>
@@ -6012,10 +6005,10 @@
       <c r="H37" s="172"/>
       <c r="I37" s="172">
         <f>SUM(I38:I42)</f>
-        <v>11628.065819672131</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" ht="15.6">
+        <v>23256.131639344261</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" ht="16" x14ac:dyDescent="0.3">
       <c r="B38" s="63">
         <v>4.0999999999999996</v>
       </c>
@@ -6027,7 +6020,7 @@
       </c>
       <c r="E38" s="165">
         <f>$E$37*D38</f>
-        <v>2.3716199999999996</v>
+        <v>4.7432399999999992</v>
       </c>
       <c r="F38" s="76">
         <v>1</v>
@@ -6041,10 +6034,10 @@
       </c>
       <c r="I38" s="171">
         <f>E38*H38*F38</f>
-        <v>315.40602049180325</v>
-      </c>
-    </row>
-    <row r="39" spans="2:11" ht="15.6">
+        <v>630.81204098360649</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" ht="16" x14ac:dyDescent="0.3">
       <c r="B39" s="63">
         <v>4.2</v>
       </c>
@@ -6056,7 +6049,7 @@
       </c>
       <c r="E39" s="165">
         <f t="shared" ref="E39:E42" si="8">$E$37*D39</f>
-        <v>11.858099999999999</v>
+        <v>23.716199999999997</v>
       </c>
       <c r="F39" s="76">
         <v>1</v>
@@ -6070,10 +6063,10 @@
       </c>
       <c r="I39" s="171">
         <f>E39*H39*F39</f>
-        <v>1577.0301024590162</v>
-      </c>
-    </row>
-    <row r="40" spans="2:11" ht="15.6">
+        <v>3154.0602049180325</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" ht="16" x14ac:dyDescent="0.3">
       <c r="B40" s="63">
         <v>4.3</v>
       </c>
@@ -6085,7 +6078,7 @@
       </c>
       <c r="E40" s="165">
         <f t="shared" si="8"/>
-        <v>15.810799999999999</v>
+        <v>31.621599999999997</v>
       </c>
       <c r="F40" s="76">
         <v>2</v>
@@ -6099,10 +6092,10 @@
       </c>
       <c r="I40" s="171">
         <f>E40*H40*F40</f>
-        <v>3217.2386065573769</v>
-      </c>
-    </row>
-    <row r="41" spans="2:11" ht="15.6">
+        <v>6434.4772131147538</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" ht="16" x14ac:dyDescent="0.3">
       <c r="B41" s="63">
         <v>4.4000000000000004</v>
       </c>
@@ -6114,7 +6107,7 @@
       </c>
       <c r="E41" s="165">
         <f t="shared" si="8"/>
-        <v>1.5810799999999998</v>
+        <v>3.1621599999999996</v>
       </c>
       <c r="F41" s="76">
         <v>1</v>
@@ -6128,10 +6121,10 @@
       </c>
       <c r="I41" s="171">
         <f t="shared" ref="I41:I42" si="9">E41*H41*F41</f>
-        <v>210.27068032786886</v>
-      </c>
-    </row>
-    <row r="42" spans="2:11" ht="15.6">
+        <v>420.54136065573772</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" ht="16" x14ac:dyDescent="0.3">
       <c r="B42" s="63">
         <v>4.5</v>
       </c>
@@ -6143,7 +6136,7 @@
       </c>
       <c r="E42" s="165">
         <f t="shared" si="8"/>
-        <v>47.432399999999994</v>
+        <v>94.864799999999988</v>
       </c>
       <c r="F42" s="76">
         <v>1</v>
@@ -6157,10 +6150,10 @@
       </c>
       <c r="I42" s="171">
         <f t="shared" si="9"/>
-        <v>6308.1204098360649</v>
-      </c>
-    </row>
-    <row r="43" spans="2:11" ht="15.6">
+        <v>12616.24081967213</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" ht="16" x14ac:dyDescent="0.3">
       <c r="B43" s="74">
         <v>5</v>
       </c>
@@ -6172,7 +6165,7 @@
       </c>
       <c r="E43" s="164">
         <f>$E$31*D43</f>
-        <v>79.053999999999988</v>
+        <v>158.10799999999998</v>
       </c>
       <c r="F43" s="88">
         <v>1</v>
@@ -6185,10 +6178,10 @@
       </c>
       <c r="I43" s="172">
         <f>SUM(I44:I47)</f>
-        <v>6289.0858913934417</v>
-      </c>
-    </row>
-    <row r="44" spans="2:11" ht="15.6">
+        <v>12578.171782786883</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" ht="16" x14ac:dyDescent="0.3">
       <c r="B44" s="140">
         <v>5.0999999999999996</v>
       </c>
@@ -6200,7 +6193,7 @@
       </c>
       <c r="E44" s="166">
         <f>$E$43*D44</f>
-        <v>11.858099999999999</v>
+        <v>23.716199999999997</v>
       </c>
       <c r="F44" s="155">
         <v>1</v>
@@ -6214,10 +6207,10 @@
       </c>
       <c r="I44" s="174">
         <f>E44*H44*F44</f>
-        <v>613.55947745901631</v>
-      </c>
-    </row>
-    <row r="45" spans="2:11" ht="15.6">
+        <v>1227.1189549180326</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" ht="16" x14ac:dyDescent="0.3">
       <c r="B45" s="63">
         <v>5.2</v>
       </c>
@@ -6229,7 +6222,7 @@
       </c>
       <c r="E45" s="166">
         <f t="shared" ref="E45:E47" si="10">$E$43*D45</f>
-        <v>19.763499999999997</v>
+        <v>39.526999999999994</v>
       </c>
       <c r="F45" s="155">
         <v>1</v>
@@ -6243,10 +6236,10 @@
       </c>
       <c r="I45" s="174">
         <f>E45*H45*F45</f>
-        <v>1146.1210040983603</v>
-      </c>
-    </row>
-    <row r="46" spans="2:11" ht="15.6">
+        <v>2292.2420081967207</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" ht="16" x14ac:dyDescent="0.3">
       <c r="B46" s="63">
         <v>5.3</v>
       </c>
@@ -6258,7 +6251,7 @@
       </c>
       <c r="E46" s="166">
         <f t="shared" si="10"/>
-        <v>23.716199999999997</v>
+        <v>47.432399999999994</v>
       </c>
       <c r="F46" s="155">
         <v>1</v>
@@ -6272,10 +6265,10 @@
       </c>
       <c r="I46" s="174">
         <f>E46*H46*F46</f>
-        <v>1375.3452049180326</v>
-      </c>
-    </row>
-    <row r="47" spans="2:11" ht="15.6">
+        <v>2750.6904098360651</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" ht="16" x14ac:dyDescent="0.3">
       <c r="B47" s="139">
         <v>5.4</v>
       </c>
@@ -6287,7 +6280,7 @@
       </c>
       <c r="E47" s="167">
         <f t="shared" si="10"/>
-        <v>23.716199999999997</v>
+        <v>47.432399999999994</v>
       </c>
       <c r="F47" s="156">
         <v>1</v>
@@ -6301,22 +6294,22 @@
       </c>
       <c r="I47" s="176">
         <f>E47*H47*F47</f>
-        <v>3154.0602049180325</v>
-      </c>
-    </row>
-    <row r="48" spans="2:11" ht="63" customHeight="1">
+        <v>6308.1204098360649</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G48" s="220" t="s">
         <v>206</v>
       </c>
       <c r="H48" s="220"/>
       <c r="I48" s="177">
         <f>SUM(I43+I37+I27+I15+I9)</f>
-        <v>375056.15139344247</v>
+        <v>750112.30278688495</v>
       </c>
       <c r="J48" s="89"/>
       <c r="K48" s="89"/>
     </row>
-    <row r="49" spans="3:9" ht="18">
+    <row r="49" spans="3:9" ht="18.7" x14ac:dyDescent="0.35">
       <c r="C49" s="75"/>
       <c r="G49" s="179">
         <v>0.5</v>
@@ -6326,10 +6319,10 @@
       </c>
       <c r="I49" s="181">
         <f>I48*G49</f>
-        <v>187528.07569672124</v>
-      </c>
-    </row>
-    <row r="50" spans="3:9" ht="18">
+        <v>375056.15139344247</v>
+      </c>
+    </row>
+    <row r="50" spans="3:9" ht="18.7" x14ac:dyDescent="0.35">
       <c r="C50" s="135"/>
       <c r="G50" s="182">
         <v>0.16</v>
@@ -6339,10 +6332,10 @@
       </c>
       <c r="I50" s="184">
         <f>(SUM(I48:I49))*G50</f>
-        <v>90013.476334426203</v>
-      </c>
-    </row>
-    <row r="51" spans="3:9" ht="21" customHeight="1">
+        <v>180026.95266885241</v>
+      </c>
+    </row>
+    <row r="51" spans="3:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G51" s="118" t="s">
         <v>23</v>
       </c>
@@ -6351,16 +6344,16 @@
       </c>
       <c r="I51" s="178">
         <f>SUM(I48:I50)</f>
-        <v>652597.70342458994</v>
-      </c>
-    </row>
-    <row r="52" spans="3:9">
+        <v>1305195.4068491799</v>
+      </c>
+    </row>
+    <row r="52" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C52" s="20"/>
       <c r="G52" s="70" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="3:9">
+    <row r="53" spans="3:9" x14ac:dyDescent="0.3">
       <c r="G53" s="70" t="s">
         <v>23</v>
       </c>
@@ -6405,20 +6398,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="13.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="12.7" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="36.75" customHeight="1" thickBot="1"/>
-    <row r="2" spans="2:5">
+    <row r="1" spans="2:5" ht="36.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="80" t="s">
         <v>210</v>
       </c>
@@ -6432,7 +6425,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="82" t="s">
         <v>163</v>
       </c>
@@ -6448,7 +6441,7 @@
         <v>132.99180327868854</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="82" t="s">
         <v>159</v>
       </c>
@@ -6464,7 +6457,7 @@
         <v>82.991803278688522</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="82" t="s">
         <v>157</v>
       </c>
@@ -6480,7 +6473,7 @@
         <v>57.991803278688522</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="82" t="s">
         <v>182</v>
       </c>
@@ -6496,7 +6489,7 @@
         <v>39.241803278688522</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="82" t="s">
         <v>177</v>
       </c>
@@ -6512,7 +6505,7 @@
         <v>101.74180327868852</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="82" t="s">
         <v>202</v>
       </c>
@@ -6528,7 +6521,7 @@
         <v>57.991803278688522</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="82" t="s">
         <v>200</v>
       </c>
@@ -6544,7 +6537,7 @@
         <v>51.741803278688522</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="13.9" thickBot="1">
+    <row r="10" spans="2:5" ht="13.35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="83" t="s">
         <v>204</v>
       </c>
@@ -6560,8 +6553,8 @@
         <v>57.991803278688522</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="13.9" thickBot="1"/>
-    <row r="12" spans="2:5" ht="13.9" thickBot="1">
+    <row r="11" spans="2:5" ht="13.35" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:5" ht="14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="85" t="s">
         <v>214</v>
       </c>
@@ -6569,7 +6562,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="2:5">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="82" t="s">
         <v>215</v>
       </c>
@@ -6577,7 +6570,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="14" spans="2:5">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="82" t="s">
         <v>216</v>
       </c>
@@ -6585,7 +6578,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="2:5">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" s="82" t="s">
         <v>217</v>
       </c>
@@ -6593,7 +6586,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="16" spans="2:5">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="82" t="s">
         <v>218</v>
       </c>
@@ -6601,7 +6594,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="82" t="s">
         <v>219</v>
       </c>
@@ -6609,7 +6602,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="82" t="s">
         <v>220</v>
       </c>
@@ -6617,7 +6610,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="13.9" thickBot="1">
+    <row r="19" spans="2:5" ht="13.35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="82" t="s">
         <v>221</v>
       </c>
@@ -6625,7 +6618,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="13.9" thickBot="1">
+    <row r="20" spans="2:5" ht="14" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="87" t="s">
         <v>222</v>
       </c>
@@ -6634,8 +6627,8 @@
         <v>17550</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="13.9" thickBot="1"/>
-    <row r="22" spans="2:5" ht="13.9" thickBot="1">
+    <row r="21" spans="2:5" ht="13.35" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:5" ht="13.35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="78" t="s">
         <v>223</v>
       </c>
@@ -6656,15 +6649,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Status xmlns="035E5738-9077-49AA-867C-265905AEBD06">Final</Status>
@@ -6679,7 +6663,20 @@
 </p:properties>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="$Resources:CType_PWS_Document(1)" ma:contentTypeID="0x0101008A98423170284BEEB635F43C3CF4E98B001A4A1163653B6846ADC5D60A25EBD429" ma:contentTypeVersion="0" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="e2271a139a2b8ee801614f6b11c48dd3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="035E5738-9077-49AA-867C-265905AEBD06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7346a5ed0265b509ea77989a5de5de18" ns2:_="">
     <xsd:import namespace="035E5738-9077-49AA-867C-265905AEBD06"/>
@@ -6763,22 +6760,45 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2CCC30F-9541-4791-B45A-F1653D3E0DD1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41BF059D-5B27-49EC-990E-9B2C61BF22F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="035E5738-9077-49AA-867C-265905AEBD06"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41BF059D-5B27-49EC-990E-9B2C61BF22F9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2CCC30F-9541-4791-B45A-F1653D3E0DD1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8B212FF-E148-4D8E-AE09-6003AD42D48C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B31A9657-F60B-4F85-99EC-12093FFD5B62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B31A9657-F60B-4F85-99EC-12093FFD5B62}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8B212FF-E148-4D8E-AE09-6003AD42D48C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="035E5738-9077-49AA-867C-265905AEBD06"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>